<commit_message>
Inject system timestamp into data for template generation
</commit_message>
<xml_diff>
--- a/templates/WorkOrder.xlsx
+++ b/templates/WorkOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgurt\source\personal\lilith-reports\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD583C8D-DE64-4BD0-83C5-850B4C0F321A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF373BB-C3F5-44CE-B181-26210D1059C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OF" sheetId="1" r:id="rId1"/>
@@ -124,12 +124,6 @@
     <t>ENVIAR T: { d.order.hasExternalWork:ifEQ(true):show('Si'):elseShow('No') }</t>
   </si>
   <si>
-    <t>ANY: {d.order.plannedDate:formatD('L'):substr(6, 10)}</t>
-  </si>
-  <si>
-    <t>ANY:  {d.order.plannedDate:formatD('L'):substr(6, 10)}</t>
-  </si>
-  <si>
     <t>{ d.phases[i].details[i].machineStatusName }</t>
   </si>
   <si>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t>{ d.phases[i+1].isExternalWork:ifEQ(true):show('Si'):elseShow('No') }</t>
+  </si>
+  <si>
+    <t>ANY: {d.now:formatD('L'):substr(6, 10)}</t>
+  </si>
+  <si>
+    <t>ANY:  {d.now:formatD('L'):substr(6, 10)}</t>
   </si>
 </sst>
 </file>
@@ -469,6 +469,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -496,6 +525,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,30 +543,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -538,13 +552,12 @@
     <xf numFmtId="14" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -557,25 +570,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,75 +1823,75 @@
       <c r="A1" s="1"/>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="43" t="s">
+      <c r="A2" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="41" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="45"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="28" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2281,50 +2281,50 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="28"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="43"/>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="31"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="31"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="46"/>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="34"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="49"/>
     </row>
     <row r="44" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2349,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322D237C-2D4C-4C87-BA57-27F48B0608B7}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,68 +2364,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56"/>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="57" t="s">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="2" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="42" t="s">
+      <c r="A2" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="41" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="45"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="48"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="49" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="32" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2433,58 +2433,58 @@
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="51" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="58" t="s">
-        <v>40</v>
+      <c r="H5" s="34" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66" t="s">
+      <c r="F6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66" t="s">
+      <c r="F7" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="35" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="60" t="s">
@@ -2492,26 +2492,21 @@
       </c>
       <c r="C8" s="60"/>
       <c r="D8" s="60"/>
-      <c r="E8" s="61" t="s">
+      <c r="E8" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="61" t="s">
+      <c r="F8" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="62" t="s">
-        <v>41</v>
+      <c r="H8" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
@@ -2520,6 +2515,11 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A3:F3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update WorkOrder.xlsx template to reflect recent changes
</commit_message>
<xml_diff>
--- a/templates/WorkOrder.xlsx
+++ b/templates/WorkOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgurt\source\personal\lilith-reports\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF373BB-C3F5-44CE-B181-26210D1059C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D70B8F2-A2D2-4727-91C3-7D562DD640E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OF" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>OF: {d.order.code}</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>ANY:  {d.now:formatD('L'):substr(6, 10)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REF: {d.order.referenceCode} {d.order.referenceDescription} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATERIAL: {d.billOfMaterials[0].referenceCode} {d.billOfMaterials[0].referenceDescription} </t>
   </si>
 </sst>
 </file>
@@ -498,6 +504,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -525,56 +558,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1042,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,230 +1829,232 @@
       <c r="A1" s="1"/>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="52"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="29" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="30"/>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="50" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="52"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="56" t="s">
+      <c r="A3" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="58"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
+    </row>
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I5" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-    </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="9"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="9"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="9"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="4"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="9"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="4"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="9"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="4"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="9"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2057,8 +2065,8 @@
       <c r="E19" s="2"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="9"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
@@ -2116,52 +2124,52 @@
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="10"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+    <row r="27" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="4"/>
       <c r="H27" s="11"/>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
+    <row r="28" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="19"/>
@@ -2171,28 +2179,28 @@
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="24"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="9"/>
       <c r="H30" s="10"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
       <c r="C32" s="23"/>
@@ -2247,7 +2255,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="22"/>
       <c r="C37" s="23"/>
@@ -2269,7 +2277,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="18.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="22"/>
       <c r="C39" s="23"/>
@@ -2280,64 +2288,62 @@
       <c r="H39" s="10"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="41" t="s">
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="43"/>
-    </row>
-    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="46"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="52"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="46"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="55"/>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="47"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="49"/>
-    </row>
-    <row r="44" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A43" s="56"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="58"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A40:I43"/>
-    <mergeCell ref="A3:F3"/>
+  <mergeCells count="8">
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A41:I43"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2347,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322D237C-2D4C-4C87-BA57-27F48B0608B7}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,152 +2370,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="65" t="s">
+      <c r="A1" s="65"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="51" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="50" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="52"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="56" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="58"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="H3" s="49"/>
+    </row>
+    <row r="4" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B5" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="31" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F5" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H5" s="32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="33" t="s">
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F6" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H6" s="34" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
+      <c r="B7" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="38"/>
       <c r="H7" s="39"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B9" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="36" t="s">
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F9" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G9" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H9" s="37" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B4:D4"/>
+  <mergeCells count="14">
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
@@ -2518,8 +2536,9 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A4:H4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>